<commit_message>
Perf: filter already existing entries during importation of certificates and identify duplication conflicts
</commit_message>
<xml_diff>
--- a/backend/web/templates/template.xlsx
+++ b/backend/web/templates/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\projects\yii2\cert-verification\backend\web\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6F90D8-26EC-4EB0-BA38-C688549D9655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9F0DA58-A2B7-4ABA-83D5-DA724CCBEE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22F4EAB6-9ECA-4EC1-8379-AB8981C6D861}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Student Name</t>
   </si>
@@ -110,13 +110,61 @@
     <t>Miss Lorenz Feeney</t>
   </si>
   <si>
-    <t>Desiree Metz</t>
-  </si>
-  <si>
-    <t>Waino Jones</t>
-  </si>
-  <si>
-    <t>Jesse Haley</t>
+    <t>8484839-ans</t>
+  </si>
+  <si>
+    <t>1484839-ans</t>
+  </si>
+  <si>
+    <t>2484839-ans</t>
+  </si>
+  <si>
+    <t>3484839-ans</t>
+  </si>
+  <si>
+    <t>248439-ans</t>
+  </si>
+  <si>
+    <t>24844839-ans</t>
+  </si>
+  <si>
+    <t>4484839-ans</t>
+  </si>
+  <si>
+    <t>5484839-ans</t>
+  </si>
+  <si>
+    <t>6484839-ans</t>
+  </si>
+  <si>
+    <t>7484839-ans</t>
+  </si>
+  <si>
+    <t>9484839-ans</t>
+  </si>
+  <si>
+    <t>10484839-ans</t>
+  </si>
+  <si>
+    <t>11484839-ans</t>
+  </si>
+  <si>
+    <t>12484839-ans</t>
+  </si>
+  <si>
+    <t>13484839-ans</t>
+  </si>
+  <si>
+    <t>14484839-ans</t>
+  </si>
+  <si>
+    <t>15484839-ans</t>
+  </si>
+  <si>
+    <t>16484839-ans</t>
+  </si>
+  <si>
+    <t>17484839-ans</t>
   </si>
 </sst>
 </file>
@@ -546,7 +594,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,10 +621,10 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45411</v>
-      </c>
-      <c r="C2">
-        <v>2307289274</v>
+        <v>45412</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -585,10 +633,10 @@
       </c>
       <c r="B3" s="3">
         <f t="shared" ref="B3:B25" ca="1" si="0">TODAY()</f>
-        <v>45411</v>
-      </c>
-      <c r="C3">
-        <v>2307289275</v>
+        <v>45412</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -597,10 +645,10 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C4">
-        <v>2307289276</v>
+        <v>45412</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -609,10 +657,10 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C5">
-        <v>2307289277</v>
+        <v>45412</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -621,10 +669,10 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C6">
-        <v>2307289278</v>
+        <v>45412</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -633,11 +681,10 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C7">
-        <f ca="1">C6+RANDBETWEEN(10,3499)</f>
-        <v>2307292163</v>
+        <v>45412</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -646,11 +693,10 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C8">
-        <f ca="1">C7+RAND()</f>
-        <v>2307292163.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -659,11 +705,10 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C9">
-        <f ca="1">C8+RANDBETWEEN(100,9494)</f>
-        <v>2307297793.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -672,11 +717,10 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C10">
-        <f t="shared" ref="C10:C25" ca="1" si="1">C9+RANDBETWEEN(100,9494)</f>
-        <v>2307299903.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -685,11 +729,10 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C11">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307303788.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -698,11 +741,10 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307304344.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -711,11 +753,10 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C13">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307313191.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -724,11 +765,10 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C14">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307313615.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -737,11 +777,10 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C15">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307316577.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -750,11 +789,10 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C16">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307316769.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -763,11 +801,10 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C17">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307321143.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -776,11 +813,10 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C18">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307321264.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -789,11 +825,10 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C19">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307328312.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -802,11 +837,10 @@
       </c>
       <c r="B20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C20">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307329874.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -815,11 +849,10 @@
       </c>
       <c r="B21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C21">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307334958.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -828,51 +861,23 @@
       </c>
       <c r="B22" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C22">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307339301.9553866</v>
+        <v>45412</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C23">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307346679.9553866</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307348260.9553866</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="3">
-        <f t="shared" ca="1" si="0"/>
-        <v>45411</v>
-      </c>
-      <c r="C25">
-        <f t="shared" ca="1" si="1"/>
-        <v>2307351154.9553866</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>

</xml_diff>